<commit_message>
ci: refacotor pacakge structure and ci init
</commit_message>
<xml_diff>
--- a/ExcelAgent/contracts.xlsx
+++ b/ExcelAgent/contracts.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
@@ -986,8 +986,6 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
           <t>Kunal</t>
@@ -998,14 +996,52 @@
           <t>Piyush</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Kunal</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Suyog</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Kunal</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Piyush</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Ek Kunal</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Piyush</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>